<commit_message>
get_comments setting working fixed write to excel file for chinese_count
</commit_message>
<xml_diff>
--- a/UGCOfMajorGames.xlsx
+++ b/UGCOfMajorGames.xlsx
@@ -22,7 +22,7 @@
     <t>Game Name</t>
   </si>
   <si>
-    <t>Amount of Workshop Items as of 2024-04-09</t>
+    <t>Amount of Workshop Items as of 2024-04-22</t>
   </si>
   <si>
     <t>Counter-Strike 2</t>
@@ -43,45 +43,51 @@
     <t>Warframe</t>
   </si>
   <si>
+    <t>Sid Meier’s Civilization® VI</t>
+  </si>
+  <si>
     <t>Unturned</t>
   </si>
   <si>
+    <t>RimWorld</t>
+  </si>
+  <si>
     <t>Hearts of Iron IV</t>
   </si>
   <si>
-    <t>Sid Meier’s Civilization® VI</t>
-  </si>
-  <si>
     <t>Don't Starve Together</t>
   </si>
   <si>
     <t>DayZ</t>
   </si>
   <si>
+    <t>tModLoader</t>
+  </si>
+  <si>
+    <t>Euro Truck Simulator 2</t>
+  </si>
+  <si>
     <t>Myth of Empires</t>
   </si>
   <si>
-    <t>Euro Truck Simulator 2</t>
-  </si>
-  <si>
-    <t>tModLoader</t>
-  </si>
-  <si>
     <t>ARK: Survival Evolved</t>
   </si>
   <si>
+    <t>Squad</t>
+  </si>
+  <si>
     <t>Mount &amp; Blade II: Bannerlord</t>
   </si>
   <si>
+    <t>Slay the Spire</t>
+  </si>
+  <si>
     <t>Left 4 Dead 2</t>
   </si>
   <si>
     <t>Project Zomboid</t>
   </si>
   <si>
-    <t>RimWorld</t>
-  </si>
-  <si>
     <t>Garry's Mod</t>
   </si>
   <si>
@@ -100,229 +106,223 @@
     <t>Crusader Kings III</t>
   </si>
   <si>
-    <t>Slay the Spire</t>
-  </si>
-  <si>
-    <t>Squad</t>
+    <t>Cities: Skylines</t>
+  </si>
+  <si>
+    <t>Rocket League®</t>
   </si>
   <si>
     <t>VTube Studio</t>
   </si>
   <si>
-    <t>Cities: Skylines</t>
-  </si>
-  <si>
-    <t>Rocket League®</t>
-  </si>
-  <si>
     <t>Stellaris</t>
   </si>
   <si>
     <t>Cookie Clicker</t>
   </si>
   <si>
+    <t>Arma 3</t>
+  </si>
+  <si>
     <t>Aimlabs</t>
   </si>
   <si>
-    <t>Arma 3</t>
+    <t>Golf With Your Friends</t>
+  </si>
+  <si>
+    <t>YoloMouse - Game Cursor Changer</t>
   </si>
   <si>
     <t>Conan Exiles</t>
   </si>
   <si>
+    <t>Brotato</t>
+  </si>
+  <si>
+    <t>Victoria 3</t>
+  </si>
+  <si>
+    <t>鬼谷八荒 Tale of Immortal</t>
+  </si>
+  <si>
     <t>Kenshi</t>
   </si>
   <si>
-    <t>Victoria 3</t>
-  </si>
-  <si>
-    <t>YoloMouse - Game Cursor Changer</t>
+    <t>DSX</t>
   </si>
   <si>
     <t>Mount &amp; Blade: Warband</t>
   </si>
   <si>
+    <t>Noita</t>
+  </si>
+  <si>
+    <t>American Truck Simulator</t>
+  </si>
+  <si>
+    <t>Dying Light</t>
+  </si>
+  <si>
+    <t>Company of Heroes 2</t>
+  </si>
+  <si>
     <t>Planet Zoo</t>
   </si>
   <si>
-    <t>Brotato</t>
-  </si>
-  <si>
-    <t>鬼谷八荒 Tale of Immortal</t>
-  </si>
-  <si>
-    <t>Dying Light</t>
-  </si>
-  <si>
-    <t>Noita</t>
-  </si>
-  <si>
     <t>People Playground</t>
   </si>
   <si>
+    <t>SAO Utils 2: Progressive</t>
+  </si>
+  <si>
     <t>Divinity: Original Sin 2 - Definitive Edition</t>
   </si>
   <si>
-    <t>Company of Heroes 2</t>
-  </si>
-  <si>
-    <t>American Truck Simulator</t>
-  </si>
-  <si>
-    <t>SAO Utils 2: Progressive</t>
+    <t>XCOM® 2</t>
+  </si>
+  <si>
+    <t>They Are Billions</t>
   </si>
   <si>
     <t>Space Engineers</t>
   </si>
   <si>
+    <t>Halo: The Master Chief Collection</t>
+  </si>
+  <si>
     <t>Dead Cells</t>
   </si>
   <si>
-    <t>They Are Billions</t>
+    <t>F1® 23</t>
+  </si>
+  <si>
+    <t>Age of Empires II (Retired)</t>
   </si>
   <si>
     <t>Tabletop Simulator</t>
   </si>
   <si>
-    <t>XCOM® 2</t>
-  </si>
-  <si>
-    <t>Age of Empires II (Retired)</t>
+    <t>Hero's Adventure: Road to Passion</t>
   </si>
   <si>
     <t>Transport Fever 2</t>
   </si>
   <si>
+    <t>Call of Duty®: Black Ops III</t>
+  </si>
+  <si>
+    <t>Farthest Frontier</t>
+  </si>
+  <si>
+    <t>Warhammer 40,000: Rogue Trader</t>
+  </si>
+  <si>
     <t>Killing Floor 2</t>
   </si>
   <si>
-    <t>DSX</t>
-  </si>
-  <si>
-    <t>F1® 23</t>
+    <t>A Dance of Fire and Ice</t>
+  </si>
+  <si>
+    <t>MyDockFinder</t>
   </si>
   <si>
     <t>X4: Foundations</t>
   </si>
   <si>
-    <t>Farthest Frontier</t>
+    <t>Total War: WARHAMMER II</t>
+  </si>
+  <si>
+    <t>SAO Utils: Beta</t>
+  </si>
+  <si>
+    <t>Pummel Party</t>
+  </si>
+  <si>
+    <t>觅长生</t>
+  </si>
+  <si>
+    <t>Company of Heroes 3</t>
+  </si>
+  <si>
+    <t>Human Fall Flat</t>
+  </si>
+  <si>
+    <t>Call to Arms - Gates of Hell: Ostfront</t>
+  </si>
+  <si>
+    <t>KovaaK's</t>
+  </si>
+  <si>
+    <t>Banana Shooter</t>
+  </si>
+  <si>
+    <t>Don't Starve</t>
+  </si>
+  <si>
+    <t>CarX Drift Racing Online</t>
+  </si>
+  <si>
+    <t>Teardown</t>
+  </si>
+  <si>
+    <t>Football Manager 2020</t>
+  </si>
+  <si>
+    <t>Barotrauma</t>
   </si>
   <si>
     <t>Stranded: Alien Dawn</t>
   </si>
   <si>
-    <t>MyDockFinder</t>
+    <t>The Elder Scrolls V: Skyrim</t>
+  </si>
+  <si>
+    <t>Songs of Syx</t>
+  </si>
+  <si>
+    <t>House Flipper</t>
+  </si>
+  <si>
+    <t>Workers &amp; Resources: Soviet Republic</t>
   </si>
   <si>
     <t>Hydroneer</t>
   </si>
   <si>
-    <t>Company of Heroes 3</t>
-  </si>
-  <si>
-    <t>觅长生</t>
-  </si>
-  <si>
-    <t>Total War: WARHAMMER II</t>
-  </si>
-  <si>
-    <t>Halo: The Master Chief Collection</t>
-  </si>
-  <si>
-    <t>SAO Utils: Beta</t>
-  </si>
-  <si>
-    <t>Call to Arms - Gates of Hell: Ostfront</t>
-  </si>
-  <si>
-    <t>A Dance of Fire and Ice</t>
-  </si>
-  <si>
-    <t>Hero's Adventure: Road to Passion</t>
-  </si>
-  <si>
-    <t>Call of Duty®: Black Ops III</t>
-  </si>
-  <si>
-    <t>Warhammer 40,000: Rogue Trader</t>
-  </si>
-  <si>
-    <t>KovaaK's</t>
-  </si>
-  <si>
-    <t>Teardown</t>
+    <t>Portal 2</t>
+  </si>
+  <si>
+    <t>Fisher Online</t>
   </si>
   <si>
     <t>PlateUp!</t>
   </si>
   <si>
-    <t>Don't Starve</t>
+    <t>Trove</t>
+  </si>
+  <si>
+    <t>Age of Mythology: Extended Edition</t>
+  </si>
+  <si>
+    <t>Wobbly Life</t>
+  </si>
+  <si>
+    <t>Kerbal Space Program</t>
   </si>
   <si>
     <t>Planet Coaster</t>
   </si>
   <si>
-    <t>Barotrauma</t>
-  </si>
-  <si>
-    <t>Portal 2</t>
-  </si>
-  <si>
-    <t>Football Manager 2020</t>
-  </si>
-  <si>
-    <t>CarX Drift Racing Online</t>
-  </si>
-  <si>
-    <t>Human Fall Flat</t>
-  </si>
-  <si>
-    <t>Fisher Online</t>
-  </si>
-  <si>
-    <t>The Elder Scrolls V: Skyrim</t>
-  </si>
-  <si>
-    <t>House Flipper</t>
+    <t>Library Of Ruina</t>
+  </si>
+  <si>
+    <t>Scrap Mechanic</t>
+  </si>
+  <si>
+    <t>Stormworks: Build and Rescue</t>
   </si>
   <si>
     <t>Age of Wonders 4</t>
-  </si>
-  <si>
-    <t>Workers &amp; Resources: Soviet Republic</t>
-  </si>
-  <si>
-    <t>Chrono Ark</t>
-  </si>
-  <si>
-    <t>Pummel Party</t>
-  </si>
-  <si>
-    <t>Kerbal Space Program</t>
-  </si>
-  <si>
-    <t>Banana Shooter</t>
-  </si>
-  <si>
-    <t>WorldBox - God Simulator</t>
-  </si>
-  <si>
-    <t>Scrap Mechanic</t>
-  </si>
-  <si>
-    <t>Age of Mythology: Extended Edition</t>
-  </si>
-  <si>
-    <t>Stormworks: Build and Rescue</t>
-  </si>
-  <si>
-    <t>Library Of Ruina</t>
-  </si>
-  <si>
-    <t>Trove</t>
-  </si>
-  <si>
-    <t>This War of Mine</t>
   </si>
   <si>
     <t>Company of Heroes</t>
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>4310</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>32694</v>
+        <v>32603</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -704,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2176571</v>
+        <v>2187431</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -715,7 +715,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>118247</v>
+        <v>118623</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -726,7 +726,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>9490</v>
+        <v>9527</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -737,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>869</v>
+        <v>881</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -748,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>101288</v>
+        <v>9316</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -759,7 +759,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>48361</v>
+        <v>101670</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -770,7 +770,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>9261</v>
+        <v>35691</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -781,7 +781,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>17102</v>
+        <v>48550</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -792,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>58067</v>
+        <v>17179</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -803,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>58704</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -814,7 +814,7 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>22266</v>
+        <v>6960</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -825,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>6892</v>
+        <v>22381</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -836,7 +836,7 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>19552</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -847,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>611</v>
+        <v>19625</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -858,7 +858,7 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>141633</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -869,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>26572</v>
+        <v>619</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -880,7 +880,7 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>35252</v>
+        <v>947</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -891,7 +891,7 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>1805952</v>
+        <v>142550</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -901,8 +901,8 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>24</v>
+      <c r="C22">
+        <v>26808</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -910,10 +910,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>598</v>
+        <v>1807968</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -921,10 +921,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
-      </c>
-      <c r="C24">
-        <v>12776</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -935,7 +935,7 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>8152</v>
+        <v>601</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -946,7 +946,7 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>940</v>
+        <v>12834</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -957,7 +957,7 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>459</v>
+        <v>8235</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -968,7 +968,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>865</v>
+        <v>340432</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -979,7 +979,7 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>339418</v>
+        <v>608</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -990,7 +990,7 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>606</v>
+        <v>874</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1001,7 +1001,7 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>29308</v>
+        <v>29413</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1012,7 +1012,7 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>1236</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1023,7 +1023,7 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>42105</v>
+        <v>144321</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1034,7 +1034,7 @@
         <v>36</v>
       </c>
       <c r="C34">
-        <v>143903</v>
+        <v>42675</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1045,7 +1045,7 @@
         <v>37</v>
       </c>
       <c r="C35">
-        <v>3887</v>
+        <v>19108</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1056,7 +1056,7 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>14630</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1067,7 +1067,7 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>4806</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1078,7 +1078,7 @@
         <v>40</v>
       </c>
       <c r="C38">
-        <v>69</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1089,7 +1089,7 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>398</v>
+        <v>4861</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1100,7 +1100,7 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>103871</v>
+        <v>9103</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1111,7 +1111,7 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>250</v>
+        <v>14736</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1122,7 +1122,7 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>9003</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1133,7 +1133,7 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>803</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1144,7 +1144,7 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>1238</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1155,7 +1155,7 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>706440</v>
+        <v>10727</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1166,7 +1166,7 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>4700</v>
+        <v>806</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1177,7 +1177,7 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>14938</v>
+        <v>14909</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1188,7 +1188,7 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>10696</v>
+        <v>104266</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1198,8 +1198,8 @@
       <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="C49" t="s">
-        <v>24</v>
+      <c r="C49">
+        <v>709113</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1209,8 +1209,8 @@
       <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C50">
-        <v>551100</v>
+      <c r="C50" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1221,7 +1221,7 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>723</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1232,7 +1232,7 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>4289</v>
+        <v>8543</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1243,7 +1243,7 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>82351</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1254,7 +1254,7 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>8503</v>
+        <v>552484</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1265,7 +1265,7 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>17413</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1276,7 +1276,7 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>12948</v>
+        <v>724</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1287,7 +1287,7 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>2998</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1298,7 +1298,7 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>17415</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1309,7 +1309,7 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>1277</v>
+        <v>82664</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1320,7 +1320,7 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>838</v>
+        <v>771</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1330,8 +1330,8 @@
       <c r="B61" t="s">
         <v>63</v>
       </c>
-      <c r="C61" t="s">
-        <v>24</v>
+      <c r="C61">
+        <v>13049</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1342,7 +1342,7 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>781</v>
+        <v>5255</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1352,8 +1352,8 @@
       <c r="B63" t="s">
         <v>65</v>
       </c>
-      <c r="C63">
-        <v>3571</v>
+      <c r="C63" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1364,7 +1364,7 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1375,7 +1375,7 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>493</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1386,7 +1386,7 @@
         <v>68</v>
       </c>
       <c r="C66">
-        <v>1500</v>
+        <v>18870</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1397,7 +1397,7 @@
         <v>69</v>
       </c>
       <c r="C67">
-        <v>12716</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1408,7 +1408,7 @@
         <v>70</v>
       </c>
       <c r="C68">
-        <v>1132</v>
+        <v>829</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1419,7 +1419,7 @@
         <v>71</v>
       </c>
       <c r="C69">
-        <v>263</v>
+        <v>12719</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1430,7 +1430,7 @@
         <v>72</v>
       </c>
       <c r="C70">
-        <v>1470</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1441,7 +1441,7 @@
         <v>73</v>
       </c>
       <c r="C71">
-        <v>18736</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1452,7 +1452,7 @@
         <v>74</v>
       </c>
       <c r="C72">
-        <v>703</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1463,7 +1463,7 @@
         <v>75</v>
       </c>
       <c r="C73">
-        <v>5227</v>
+        <v>509</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1474,7 +1474,7 @@
         <v>76</v>
       </c>
       <c r="C74">
-        <v>14</v>
+        <v>504748</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1485,7 +1485,7 @@
         <v>77</v>
       </c>
       <c r="C75">
-        <v>31721</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1496,7 +1496,7 @@
         <v>78</v>
       </c>
       <c r="C76">
-        <v>6555</v>
+        <v>32435</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1507,7 +1507,7 @@
         <v>79</v>
       </c>
       <c r="C77">
-        <v>260</v>
+        <v>968</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1518,7 +1518,7 @@
         <v>80</v>
       </c>
       <c r="C78">
-        <v>3201</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1529,7 +1529,7 @@
         <v>81</v>
       </c>
       <c r="C79">
-        <v>408153</v>
+        <v>870</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1540,7 +1540,7 @@
         <v>82</v>
       </c>
       <c r="C80">
-        <v>54075</v>
+        <v>6652</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1551,7 +1551,7 @@
         <v>83</v>
       </c>
       <c r="C81">
-        <v>947122</v>
+        <v>20132</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1562,7 +1562,7 @@
         <v>84</v>
       </c>
       <c r="C82">
-        <v>20129</v>
+        <v>54353</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1573,7 +1573,7 @@
         <v>85</v>
       </c>
       <c r="C83">
-        <v>852</v>
+        <v>786</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1584,7 +1584,7 @@
         <v>86</v>
       </c>
       <c r="C84">
-        <v>503928</v>
+        <v>27731</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1595,7 +1595,7 @@
         <v>87</v>
       </c>
       <c r="C85">
-        <v>568</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1606,7 +1606,7 @@
         <v>88</v>
       </c>
       <c r="C86">
-        <v>27740</v>
+        <v>30089</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1617,7 +1617,7 @@
         <v>89</v>
       </c>
       <c r="C87">
-        <v>29793</v>
+        <v>9163</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1628,7 +1628,7 @@
         <v>90</v>
       </c>
       <c r="C88">
-        <v>696</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1639,7 +1639,7 @@
         <v>91</v>
       </c>
       <c r="C89">
-        <v>9119</v>
+        <v>948465</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1650,7 +1650,7 @@
         <v>92</v>
       </c>
       <c r="C90">
-        <v>161</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1661,7 +1661,7 @@
         <v>93</v>
       </c>
       <c r="C91">
-        <v>1327</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1672,7 +1672,7 @@
         <v>94</v>
       </c>
       <c r="C92">
-        <v>105353</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1683,7 +1683,7 @@
         <v>95</v>
       </c>
       <c r="C93">
-        <v>953</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1694,7 +1694,7 @@
         <v>96</v>
       </c>
       <c r="C94">
-        <v>64031</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1705,7 +1705,7 @@
         <v>97</v>
       </c>
       <c r="C95">
-        <v>479102</v>
+        <v>105595</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1716,7 +1716,7 @@
         <v>98</v>
       </c>
       <c r="C96">
-        <v>2222</v>
+        <v>408730</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1727,7 +1727,7 @@
         <v>99</v>
       </c>
       <c r="C97">
-        <v>245356</v>
+        <v>5920</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1738,7 +1738,7 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>5905</v>
+        <v>480190</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1749,7 +1749,7 @@
         <v>101</v>
       </c>
       <c r="C99">
-        <v>2188</v>
+        <v>246550</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1760,7 +1760,7 @@
         <v>102</v>
       </c>
       <c r="C100">
-        <v>13218</v>
+        <v>719</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1771,7 +1771,7 @@
         <v>103</v>
       </c>
       <c r="C101">
-        <v>3345</v>
+        <v>3337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>